<commit_message>
add item selection rationale
</commit_message>
<xml_diff>
--- a/Materials/BANGS.xlsx
+++ b/Materials/BANGS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Desktop/Research/3 Submitted Projects/2022 BANG Questionnaire/Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AAEA5F-A504-004B-ACCF-CC63DDBF73B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C875B903-A57B-284D-9536-ED5C83121FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2340" windowWidth="27640" windowHeight="16940" xr2:uid="{43670338-F45A-5B4E-AEA1-2D0A6DACD0A3}"/>
+    <workbookView xWindow="5340" yWindow="1900" windowWidth="27640" windowHeight="16940" xr2:uid="{43670338-F45A-5B4E-AEA1-2D0A6DACD0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1447,7 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AE0C6A-4BE2-1948-BCE8-C3527ECCDD8B}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:C51"/>
     </sheetView>
   </sheetViews>

</xml_diff>